<commit_message>
Add introductions to schedule
</commit_message>
<xml_diff>
--- a/en/schedule/schedule.xlsx
+++ b/en/schedule/schedule.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Break</t>
   </si>
@@ -774,6 +774,22 @@
       </rPr>
       <t xml:space="preserve">
 Room - Jean-Despréz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Opening and Introductions
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Room - Salle des Fêtes</t>
     </r>
   </si>
 </sst>
@@ -878,7 +894,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -901,8 +917,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -928,8 +981,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -958,8 +1013,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -972,6 +1036,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -984,6 +1049,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1316,10 +1382,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1339,189 +1405,201 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="99" customHeight="1" thickBot="1">
+    <row r="2" spans="1:5" ht="42" customHeight="1" thickBot="1">
       <c r="A2" s="3">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" ht="99" customHeight="1" thickBot="1">
+      <c r="A3" s="3">
         <v>0.375</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A3" s="3">
+    <row r="4" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A4" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="115" thickBot="1">
-      <c r="A4" s="3">
+    <row r="5" spans="1:5" ht="115" thickBot="1">
+      <c r="A5" s="3">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A5" s="3">
+    <row r="6" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A6" s="3">
         <v>0.46875</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="145" thickBot="1">
-      <c r="A6" s="3">
+    <row r="7" spans="1:5" ht="145" thickBot="1">
+      <c r="A7" s="3">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A7" s="3">
+    <row r="8" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A8" s="3">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="67" customHeight="1" thickBot="1">
-      <c r="A8" s="3">
+    <row r="9" spans="1:5" ht="67" customHeight="1" thickBot="1">
+      <c r="A9" s="3">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
-    <row r="9" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A9" s="3">
+    <row r="10" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A10" s="3">
         <v>9.375E-2</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="169" thickBot="1">
-      <c r="A10" s="3">
+    <row r="11" spans="1:5" ht="169" thickBot="1">
+      <c r="A11" s="3">
         <v>0.10416666666666667</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A11" s="3">
+    <row r="12" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A12" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="115" thickBot="1">
-      <c r="A12" s="3">
+    <row r="13" spans="1:5" ht="115" thickBot="1">
+      <c r="A13" s="3">
         <v>0.17708333333333334</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="3">
+    <row r="14" spans="1:5" ht="36" customHeight="1" thickBot="1">
+      <c r="A14" s="3">
         <v>0.21875</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="25" customHeight="1" thickBot="1">
-      <c r="A14" s="3">
+    <row r="15" spans="1:5" ht="25" customHeight="1" thickBot="1">
+      <c r="A15" s="3">
         <v>0.23958333333333334</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="70" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
+  <pageSetup scale="72" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>